<commit_message>
update to initial spreadsheet members and payment
</commit_message>
<xml_diff>
--- a/WELFARE FINANCE DATA 2016 updated.xlsx
+++ b/WELFARE FINANCE DATA 2016 updated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="1237">
   <si>
     <t xml:space="preserve">Membership Number</t>
   </si>
@@ -3732,6 +3732,15 @@
   </si>
   <si>
     <t xml:space="preserve">SHIBANDU ROBERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PATRICK MURIITHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NICODEMUS M NDUYA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHOLASTICA N.MUTINDA</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -3915,7 +3924,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3992,15 +4001,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11273,20 +11274,20 @@
   </sheetPr>
   <dimension ref="A1:O165"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A119" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A132" activeCellId="0" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="7.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="8" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="8" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="6.43"/>
@@ -11636,7 +11637,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>1017</v>
+        <v>1233</v>
       </c>
       <c r="B10" s="8" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -13410,7 +13411,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="8" t="s">
-        <v>1130</v>
+        <v>1234</v>
       </c>
       <c r="B131" s="8" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -13514,7 +13515,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="8" t="s">
-        <v>1161</v>
+        <v>1235</v>
       </c>
       <c r="B139" s="8" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -13893,10 +13894,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.28"/>
@@ -20958,10 +20959,10 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="4.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="3.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="2.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="2.71"/>
@@ -20969,7 +20970,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="8" width="4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="8" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="8" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.43"/>
@@ -39136,12 +39137,12 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="7.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="8" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="8" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="6.43"/>
@@ -40843,8 +40844,8 @@
   </sheetPr>
   <dimension ref="A1:AH185"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40855,10 +40856,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.28"/>
@@ -41355,7 +41356,7 @@
       <c r="K8" s="8" t="n">
         <v>200</v>
       </c>
-      <c r="L8" s="19" t="n">
+      <c r="L8" s="11" t="n">
         <v>200</v>
       </c>
       <c r="M8" s="8" t="n">
@@ -41990,7 +41991,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>1017</v>
+        <v>1233</v>
       </c>
       <c r="B18" s="8" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -42320,7 +42321,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>1130</v>
+        <v>1234</v>
       </c>
       <c r="B23" s="8" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -42383,7 +42384,7 @@
       <c r="AD23" s="8"/>
       <c r="AE23" s="8"/>
       <c r="AF23" s="8"/>
-      <c r="AG23" s="20"/>
+      <c r="AG23" s="19"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
@@ -42450,7 +42451,7 @@
       <c r="AD24" s="8"/>
       <c r="AE24" s="8"/>
       <c r="AF24" s="8"/>
-      <c r="AG24" s="20"/>
+      <c r="AG24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
@@ -42517,7 +42518,7 @@
       <c r="AD25" s="8"/>
       <c r="AE25" s="8"/>
       <c r="AF25" s="8"/>
-      <c r="AG25" s="20"/>
+      <c r="AG25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
@@ -42584,7 +42585,7 @@
       <c r="AD26" s="8"/>
       <c r="AE26" s="8"/>
       <c r="AF26" s="8"/>
-      <c r="AG26" s="20"/>
+      <c r="AG26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
@@ -42651,7 +42652,7 @@
       <c r="AD27" s="8"/>
       <c r="AE27" s="8"/>
       <c r="AF27" s="8"/>
-      <c r="AG27" s="20"/>
+      <c r="AG27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
@@ -42718,7 +42719,7 @@
       <c r="AD28" s="8"/>
       <c r="AE28" s="8"/>
       <c r="AF28" s="8"/>
-      <c r="AG28" s="20"/>
+      <c r="AG28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
@@ -42785,7 +42786,7 @@
       <c r="AD29" s="8"/>
       <c r="AE29" s="8"/>
       <c r="AF29" s="8"/>
-      <c r="AG29" s="20"/>
+      <c r="AG29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
@@ -42852,7 +42853,7 @@
       <c r="AD30" s="8"/>
       <c r="AE30" s="8"/>
       <c r="AF30" s="8"/>
-      <c r="AG30" s="20"/>
+      <c r="AG30" s="19"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
@@ -42919,7 +42920,7 @@
       <c r="AD31" s="9"/>
       <c r="AE31" s="9"/>
       <c r="AF31" s="9"/>
-      <c r="AG31" s="20"/>
+      <c r="AG31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
@@ -43055,7 +43056,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>1161</v>
+        <v>1235</v>
       </c>
       <c r="B34" s="8" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -43659,12 +43660,12 @@
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
       <c r="T43" s="8"/>
-      <c r="U43" s="20"/>
-      <c r="V43" s="20"/>
-      <c r="W43" s="20"/>
-      <c r="X43" s="20"/>
-      <c r="Y43" s="20"/>
-      <c r="Z43" s="20"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="19"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="19"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
@@ -43699,7 +43700,7 @@
         <v>100</v>
       </c>
       <c r="K44" s="8"/>
-      <c r="L44" s="21"/>
+      <c r="L44" s="13"/>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
       <c r="O44" s="18" t="n">
@@ -43711,12 +43712,12 @@
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
       <c r="T44" s="8"/>
-      <c r="U44" s="20"/>
-      <c r="V44" s="20"/>
-      <c r="W44" s="20"/>
-      <c r="X44" s="20"/>
-      <c r="Y44" s="20"/>
-      <c r="Z44" s="20"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+      <c r="Y44" s="19"/>
+      <c r="Z44" s="19"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
@@ -43763,12 +43764,12 @@
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
       <c r="T45" s="8"/>
-      <c r="U45" s="20"/>
-      <c r="V45" s="20"/>
-      <c r="W45" s="20"/>
-      <c r="X45" s="20"/>
-      <c r="Y45" s="20"/>
-      <c r="Z45" s="20"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="19"/>
+      <c r="W45" s="19"/>
+      <c r="X45" s="19"/>
+      <c r="Y45" s="19"/>
+      <c r="Z45" s="19"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
@@ -43813,12 +43814,12 @@
       <c r="R46" s="8"/>
       <c r="S46" s="8"/>
       <c r="T46" s="8"/>
-      <c r="U46" s="20"/>
-      <c r="V46" s="20"/>
-      <c r="W46" s="20"/>
-      <c r="X46" s="20"/>
-      <c r="Y46" s="20"/>
-      <c r="Z46" s="20"/>
+      <c r="U46" s="19"/>
+      <c r="V46" s="19"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="19"/>
+      <c r="Y46" s="19"/>
+      <c r="Z46" s="19"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
@@ -43849,9 +43850,9 @@
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="K47" s="9"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
       <c r="O47" s="18" t="n">
         <f aca="false">SUM(C47:N47)</f>
         <v>1200</v>
@@ -43861,12 +43862,12 @@
       <c r="R47" s="8"/>
       <c r="S47" s="8"/>
       <c r="T47" s="8"/>
-      <c r="U47" s="20"/>
-      <c r="V47" s="20"/>
-      <c r="W47" s="20"/>
-      <c r="X47" s="20"/>
-      <c r="Y47" s="20"/>
-      <c r="Z47" s="20"/>
+      <c r="U47" s="19"/>
+      <c r="V47" s="19"/>
+      <c r="W47" s="19"/>
+      <c r="X47" s="19"/>
+      <c r="Y47" s="19"/>
+      <c r="Z47" s="19"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
@@ -43907,12 +43908,12 @@
       <c r="R48" s="8"/>
       <c r="S48" s="8"/>
       <c r="T48" s="8"/>
-      <c r="U48" s="20"/>
-      <c r="V48" s="20"/>
-      <c r="W48" s="20"/>
-      <c r="X48" s="20"/>
-      <c r="Y48" s="20"/>
-      <c r="Z48" s="20"/>
+      <c r="U48" s="19"/>
+      <c r="V48" s="19"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="19"/>
+      <c r="Y48" s="19"/>
+      <c r="Z48" s="19"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
@@ -43953,12 +43954,12 @@
       <c r="R49" s="8"/>
       <c r="S49" s="8"/>
       <c r="T49" s="8"/>
-      <c r="U49" s="20"/>
-      <c r="V49" s="20"/>
-      <c r="W49" s="20"/>
-      <c r="X49" s="20"/>
-      <c r="Y49" s="20"/>
-      <c r="Z49" s="20"/>
+      <c r="U49" s="19"/>
+      <c r="V49" s="19"/>
+      <c r="W49" s="19"/>
+      <c r="X49" s="19"/>
+      <c r="Y49" s="19"/>
+      <c r="Z49" s="19"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
@@ -43999,12 +44000,12 @@
       <c r="R50" s="8"/>
       <c r="S50" s="8"/>
       <c r="T50" s="8"/>
-      <c r="U50" s="20"/>
-      <c r="V50" s="20"/>
-      <c r="W50" s="20"/>
-      <c r="X50" s="20"/>
-      <c r="Y50" s="20"/>
-      <c r="Z50" s="20"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="19"/>
+      <c r="Y50" s="19"/>
+      <c r="Z50" s="19"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
@@ -44045,12 +44046,12 @@
       <c r="R51" s="8"/>
       <c r="S51" s="8"/>
       <c r="T51" s="8"/>
-      <c r="U51" s="20"/>
-      <c r="V51" s="20"/>
-      <c r="W51" s="20"/>
-      <c r="X51" s="20"/>
-      <c r="Y51" s="20"/>
-      <c r="Z51" s="20"/>
+      <c r="U51" s="19"/>
+      <c r="V51" s="19"/>
+      <c r="W51" s="19"/>
+      <c r="X51" s="19"/>
+      <c r="Y51" s="19"/>
+      <c r="Z51" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
@@ -44091,12 +44092,12 @@
       <c r="R52" s="8"/>
       <c r="S52" s="8"/>
       <c r="T52" s="8"/>
-      <c r="U52" s="20"/>
-      <c r="V52" s="20"/>
-      <c r="W52" s="20"/>
-      <c r="X52" s="20"/>
-      <c r="Y52" s="20"/>
-      <c r="Z52" s="20"/>
+      <c r="U52" s="19"/>
+      <c r="V52" s="19"/>
+      <c r="W52" s="19"/>
+      <c r="X52" s="19"/>
+      <c r="Y52" s="19"/>
+      <c r="Z52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="s">
@@ -44130,17 +44131,17 @@
         <f aca="false">SUM(C53:N53)</f>
         <v>800</v>
       </c>
-      <c r="P53" s="20"/>
-      <c r="Q53" s="20"/>
-      <c r="R53" s="20"/>
-      <c r="S53" s="20"/>
-      <c r="T53" s="20"/>
-      <c r="U53" s="20"/>
-      <c r="V53" s="20"/>
-      <c r="W53" s="20"/>
-      <c r="X53" s="20"/>
-      <c r="Y53" s="20"/>
-      <c r="Z53" s="20"/>
+      <c r="P53" s="19"/>
+      <c r="Q53" s="19"/>
+      <c r="R53" s="19"/>
+      <c r="S53" s="19"/>
+      <c r="T53" s="19"/>
+      <c r="U53" s="19"/>
+      <c r="V53" s="19"/>
+      <c r="W53" s="19"/>
+      <c r="X53" s="19"/>
+      <c r="Y53" s="19"/>
+      <c r="Z53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
@@ -44183,10 +44184,10 @@
       <c r="X54" s="8"/>
       <c r="Y54" s="8"/>
       <c r="Z54" s="8"/>
-      <c r="AA54" s="20"/>
-      <c r="AB54" s="20"/>
-      <c r="AC54" s="20"/>
-      <c r="AD54" s="20"/>
+      <c r="AA54" s="19"/>
+      <c r="AB54" s="19"/>
+      <c r="AC54" s="19"/>
+      <c r="AD54" s="19"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
@@ -44229,10 +44230,10 @@
       <c r="X55" s="8"/>
       <c r="Y55" s="8"/>
       <c r="Z55" s="8"/>
-      <c r="AA55" s="20"/>
-      <c r="AB55" s="20"/>
-      <c r="AC55" s="20"/>
-      <c r="AD55" s="20"/>
+      <c r="AA55" s="19"/>
+      <c r="AB55" s="19"/>
+      <c r="AC55" s="19"/>
+      <c r="AD55" s="19"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="s">
@@ -44275,10 +44276,10 @@
       <c r="X56" s="8"/>
       <c r="Y56" s="8"/>
       <c r="Z56" s="8"/>
-      <c r="AA56" s="20"/>
-      <c r="AB56" s="20"/>
-      <c r="AC56" s="20"/>
-      <c r="AD56" s="20"/>
+      <c r="AA56" s="19"/>
+      <c r="AB56" s="19"/>
+      <c r="AC56" s="19"/>
+      <c r="AD56" s="19"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
@@ -44319,10 +44320,10 @@
       <c r="X57" s="8"/>
       <c r="Y57" s="8"/>
       <c r="Z57" s="8"/>
-      <c r="AA57" s="20"/>
-      <c r="AB57" s="20"/>
-      <c r="AC57" s="20"/>
-      <c r="AD57" s="20"/>
+      <c r="AA57" s="19"/>
+      <c r="AB57" s="19"/>
+      <c r="AC57" s="19"/>
+      <c r="AD57" s="19"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
@@ -44363,10 +44364,10 @@
       <c r="X58" s="8"/>
       <c r="Y58" s="8"/>
       <c r="Z58" s="8"/>
-      <c r="AA58" s="20"/>
-      <c r="AB58" s="20"/>
-      <c r="AC58" s="20"/>
-      <c r="AD58" s="20"/>
+      <c r="AA58" s="19"/>
+      <c r="AB58" s="19"/>
+      <c r="AC58" s="19"/>
+      <c r="AD58" s="19"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
@@ -44407,10 +44408,10 @@
       <c r="X59" s="8"/>
       <c r="Y59" s="8"/>
       <c r="Z59" s="8"/>
-      <c r="AA59" s="20"/>
-      <c r="AB59" s="20"/>
-      <c r="AC59" s="20"/>
-      <c r="AD59" s="20"/>
+      <c r="AA59" s="19"/>
+      <c r="AB59" s="19"/>
+      <c r="AC59" s="19"/>
+      <c r="AD59" s="19"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
@@ -44451,10 +44452,10 @@
       <c r="X60" s="8"/>
       <c r="Y60" s="8"/>
       <c r="Z60" s="8"/>
-      <c r="AA60" s="20"/>
-      <c r="AB60" s="20"/>
-      <c r="AC60" s="20"/>
-      <c r="AD60" s="20"/>
+      <c r="AA60" s="19"/>
+      <c r="AB60" s="19"/>
+      <c r="AC60" s="19"/>
+      <c r="AD60" s="19"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
@@ -44495,10 +44496,10 @@
       <c r="X61" s="8"/>
       <c r="Y61" s="8"/>
       <c r="Z61" s="8"/>
-      <c r="AA61" s="20"/>
-      <c r="AB61" s="20"/>
-      <c r="AC61" s="20"/>
-      <c r="AD61" s="20"/>
+      <c r="AA61" s="19"/>
+      <c r="AB61" s="19"/>
+      <c r="AC61" s="19"/>
+      <c r="AD61" s="19"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8" t="s">
@@ -44539,10 +44540,10 @@
       <c r="X62" s="8"/>
       <c r="Y62" s="8"/>
       <c r="Z62" s="8"/>
-      <c r="AA62" s="20"/>
-      <c r="AB62" s="20"/>
-      <c r="AC62" s="20"/>
-      <c r="AD62" s="20"/>
+      <c r="AA62" s="19"/>
+      <c r="AB62" s="19"/>
+      <c r="AC62" s="19"/>
+      <c r="AD62" s="19"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
@@ -44583,10 +44584,10 @@
       <c r="X63" s="8"/>
       <c r="Y63" s="8"/>
       <c r="Z63" s="8"/>
-      <c r="AA63" s="20"/>
-      <c r="AB63" s="20"/>
-      <c r="AC63" s="20"/>
-      <c r="AD63" s="20"/>
+      <c r="AA63" s="19"/>
+      <c r="AB63" s="19"/>
+      <c r="AC63" s="19"/>
+      <c r="AD63" s="19"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8" t="s">
@@ -44627,10 +44628,10 @@
       <c r="X64" s="8"/>
       <c r="Y64" s="8"/>
       <c r="Z64" s="8"/>
-      <c r="AA64" s="20"/>
-      <c r="AB64" s="20"/>
-      <c r="AC64" s="20"/>
-      <c r="AD64" s="20"/>
+      <c r="AA64" s="19"/>
+      <c r="AB64" s="19"/>
+      <c r="AC64" s="19"/>
+      <c r="AD64" s="19"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8" t="s">
@@ -44669,10 +44670,10 @@
       <c r="X65" s="8"/>
       <c r="Y65" s="8"/>
       <c r="Z65" s="8"/>
-      <c r="AA65" s="20"/>
-      <c r="AB65" s="20"/>
-      <c r="AC65" s="20"/>
-      <c r="AD65" s="20"/>
+      <c r="AA65" s="19"/>
+      <c r="AB65" s="19"/>
+      <c r="AC65" s="19"/>
+      <c r="AD65" s="19"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8" t="s">
@@ -44711,10 +44712,10 @@
       <c r="X66" s="8"/>
       <c r="Y66" s="8"/>
       <c r="Z66" s="8"/>
-      <c r="AA66" s="20"/>
-      <c r="AB66" s="20"/>
-      <c r="AC66" s="20"/>
-      <c r="AD66" s="20"/>
+      <c r="AA66" s="19"/>
+      <c r="AB66" s="19"/>
+      <c r="AC66" s="19"/>
+      <c r="AD66" s="19"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8" t="s">
@@ -44753,10 +44754,10 @@
       <c r="X67" s="8"/>
       <c r="Y67" s="8"/>
       <c r="Z67" s="8"/>
-      <c r="AA67" s="20"/>
-      <c r="AB67" s="20"/>
-      <c r="AC67" s="20"/>
-      <c r="AD67" s="20"/>
+      <c r="AA67" s="19"/>
+      <c r="AB67" s="19"/>
+      <c r="AC67" s="19"/>
+      <c r="AD67" s="19"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="8" t="s">
@@ -44795,10 +44796,10 @@
       <c r="X68" s="8"/>
       <c r="Y68" s="8"/>
       <c r="Z68" s="8"/>
-      <c r="AA68" s="20"/>
-      <c r="AB68" s="20"/>
-      <c r="AC68" s="20"/>
-      <c r="AD68" s="20"/>
+      <c r="AA68" s="19"/>
+      <c r="AB68" s="19"/>
+      <c r="AC68" s="19"/>
+      <c r="AD68" s="19"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="8" t="s">
@@ -44837,10 +44838,10 @@
       <c r="X69" s="8"/>
       <c r="Y69" s="8"/>
       <c r="Z69" s="8"/>
-      <c r="AA69" s="20"/>
-      <c r="AB69" s="20"/>
-      <c r="AC69" s="20"/>
-      <c r="AD69" s="20"/>
+      <c r="AA69" s="19"/>
+      <c r="AB69" s="19"/>
+      <c r="AC69" s="19"/>
+      <c r="AD69" s="19"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="8" t="s">
@@ -45945,10 +45946,10 @@
       <c r="AB96" s="8"/>
       <c r="AC96" s="8"/>
       <c r="AD96" s="8"/>
-      <c r="AE96" s="20"/>
-      <c r="AF96" s="20"/>
-      <c r="AG96" s="20"/>
-      <c r="AH96" s="20"/>
+      <c r="AE96" s="19"/>
+      <c r="AF96" s="19"/>
+      <c r="AG96" s="19"/>
+      <c r="AH96" s="19"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="8" t="s">
@@ -45989,10 +45990,10 @@
       <c r="AB97" s="8"/>
       <c r="AC97" s="8"/>
       <c r="AD97" s="8"/>
-      <c r="AE97" s="20"/>
-      <c r="AF97" s="20"/>
-      <c r="AG97" s="20"/>
-      <c r="AH97" s="20"/>
+      <c r="AE97" s="19"/>
+      <c r="AF97" s="19"/>
+      <c r="AG97" s="19"/>
+      <c r="AH97" s="19"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="8" t="s">
@@ -46033,10 +46034,10 @@
       <c r="AB98" s="8"/>
       <c r="AC98" s="8"/>
       <c r="AD98" s="8"/>
-      <c r="AE98" s="20"/>
-      <c r="AF98" s="20"/>
-      <c r="AG98" s="20"/>
-      <c r="AH98" s="20"/>
+      <c r="AE98" s="19"/>
+      <c r="AF98" s="19"/>
+      <c r="AG98" s="19"/>
+      <c r="AH98" s="19"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="8" t="s">
@@ -46077,10 +46078,10 @@
       <c r="AB99" s="8"/>
       <c r="AC99" s="8"/>
       <c r="AD99" s="8"/>
-      <c r="AE99" s="20"/>
-      <c r="AF99" s="20"/>
-      <c r="AG99" s="20"/>
-      <c r="AH99" s="20"/>
+      <c r="AE99" s="19"/>
+      <c r="AF99" s="19"/>
+      <c r="AG99" s="19"/>
+      <c r="AH99" s="19"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="8" t="s">
@@ -46121,10 +46122,10 @@
       <c r="AB100" s="8"/>
       <c r="AC100" s="8"/>
       <c r="AD100" s="8"/>
-      <c r="AE100" s="20"/>
-      <c r="AF100" s="20"/>
-      <c r="AG100" s="20"/>
-      <c r="AH100" s="20"/>
+      <c r="AE100" s="19"/>
+      <c r="AF100" s="19"/>
+      <c r="AG100" s="19"/>
+      <c r="AH100" s="19"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="8" t="s">
@@ -46165,8 +46166,8 @@
       <c r="AB101" s="8"/>
       <c r="AC101" s="8"/>
       <c r="AD101" s="8"/>
-      <c r="AE101" s="20"/>
-      <c r="AF101" s="20"/>
+      <c r="AE101" s="19"/>
+      <c r="AF101" s="19"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="8" t="s">
@@ -46207,8 +46208,8 @@
       <c r="AB102" s="8"/>
       <c r="AC102" s="8"/>
       <c r="AD102" s="8"/>
-      <c r="AE102" s="20"/>
-      <c r="AF102" s="20"/>
+      <c r="AE102" s="19"/>
+      <c r="AF102" s="19"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="8" t="s">
@@ -46249,8 +46250,8 @@
       <c r="AB103" s="8"/>
       <c r="AC103" s="8"/>
       <c r="AD103" s="8"/>
-      <c r="AE103" s="20"/>
-      <c r="AF103" s="20"/>
+      <c r="AE103" s="19"/>
+      <c r="AF103" s="19"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="8" t="s">
@@ -46291,8 +46292,8 @@
       <c r="AB104" s="8"/>
       <c r="AC104" s="8"/>
       <c r="AD104" s="8"/>
-      <c r="AE104" s="20"/>
-      <c r="AF104" s="20"/>
+      <c r="AE104" s="19"/>
+      <c r="AF104" s="19"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="8" t="s">
@@ -46333,9 +46334,9 @@
       <c r="AB105" s="8"/>
       <c r="AC105" s="8"/>
       <c r="AD105" s="8"/>
-      <c r="AE105" s="20"/>
-      <c r="AF105" s="20"/>
-      <c r="AG105" s="20"/>
+      <c r="AE105" s="19"/>
+      <c r="AF105" s="19"/>
+      <c r="AG105" s="19"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="8" t="s">
@@ -46376,9 +46377,9 @@
       <c r="AB106" s="8"/>
       <c r="AC106" s="8"/>
       <c r="AD106" s="8"/>
-      <c r="AE106" s="20"/>
-      <c r="AF106" s="20"/>
-      <c r="AG106" s="20"/>
+      <c r="AE106" s="19"/>
+      <c r="AF106" s="19"/>
+      <c r="AG106" s="19"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8" t="s">
@@ -47932,13 +47933,13 @@
       <c r="U145" s="8"/>
       <c r="V145" s="8"/>
       <c r="W145" s="8"/>
-      <c r="X145" s="20"/>
-      <c r="Y145" s="20"/>
-      <c r="Z145" s="20"/>
-      <c r="AA145" s="20"/>
-      <c r="AB145" s="20"/>
-      <c r="AC145" s="20"/>
-      <c r="AD145" s="20"/>
+      <c r="X145" s="19"/>
+      <c r="Y145" s="19"/>
+      <c r="Z145" s="19"/>
+      <c r="AA145" s="19"/>
+      <c r="AB145" s="19"/>
+      <c r="AC145" s="19"/>
+      <c r="AD145" s="19"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="8" t="s">
@@ -48692,14 +48693,14 @@
   </sheetPr>
   <dimension ref="A1:BE1096"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P5" activeCellId="0" sqref="P5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="30.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="7.57"/>
@@ -49819,7 +49820,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>1198</v>
+        <v>1233</v>
       </c>
       <c r="B17" s="15" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -51156,28 +51157,28 @@
       <c r="AG36" s="8"/>
       <c r="AH36" s="8"/>
       <c r="AI36" s="8"/>
-      <c r="AJ36" s="20"/>
-      <c r="AK36" s="20"/>
-      <c r="AL36" s="20"/>
-      <c r="AM36" s="20"/>
-      <c r="AN36" s="20"/>
-      <c r="AO36" s="20"/>
-      <c r="AP36" s="20"/>
-      <c r="AQ36" s="20"/>
-      <c r="AR36" s="20"/>
-      <c r="AS36" s="20"/>
-      <c r="AT36" s="20"/>
-      <c r="AU36" s="20"/>
-      <c r="AV36" s="20"/>
-      <c r="AW36" s="20"/>
-      <c r="AX36" s="20"/>
-      <c r="AY36" s="20"/>
-      <c r="AZ36" s="20"/>
-      <c r="BA36" s="20"/>
-      <c r="BB36" s="20"/>
-      <c r="BC36" s="20"/>
-      <c r="BD36" s="20"/>
-      <c r="BE36" s="20"/>
+      <c r="AJ36" s="19"/>
+      <c r="AK36" s="19"/>
+      <c r="AL36" s="19"/>
+      <c r="AM36" s="19"/>
+      <c r="AN36" s="19"/>
+      <c r="AO36" s="19"/>
+      <c r="AP36" s="19"/>
+      <c r="AQ36" s="19"/>
+      <c r="AR36" s="19"/>
+      <c r="AS36" s="19"/>
+      <c r="AT36" s="19"/>
+      <c r="AU36" s="19"/>
+      <c r="AV36" s="19"/>
+      <c r="AW36" s="19"/>
+      <c r="AX36" s="19"/>
+      <c r="AY36" s="19"/>
+      <c r="AZ36" s="19"/>
+      <c r="BA36" s="19"/>
+      <c r="BB36" s="19"/>
+      <c r="BC36" s="19"/>
+      <c r="BD36" s="19"/>
+      <c r="BE36" s="19"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
@@ -51233,28 +51234,28 @@
       <c r="AG37" s="8"/>
       <c r="AH37" s="8"/>
       <c r="AI37" s="8"/>
-      <c r="AJ37" s="20"/>
-      <c r="AK37" s="20"/>
-      <c r="AL37" s="20"/>
-      <c r="AM37" s="20"/>
-      <c r="AN37" s="20"/>
-      <c r="AO37" s="20"/>
-      <c r="AP37" s="20"/>
-      <c r="AQ37" s="20"/>
-      <c r="AR37" s="20"/>
-      <c r="AS37" s="20"/>
-      <c r="AT37" s="20"/>
-      <c r="AU37" s="20"/>
-      <c r="AV37" s="20"/>
-      <c r="AW37" s="20"/>
-      <c r="AX37" s="20"/>
-      <c r="AY37" s="20"/>
-      <c r="AZ37" s="20"/>
-      <c r="BA37" s="20"/>
-      <c r="BB37" s="20"/>
-      <c r="BC37" s="20"/>
-      <c r="BD37" s="20"/>
-      <c r="BE37" s="20"/>
+      <c r="AJ37" s="19"/>
+      <c r="AK37" s="19"/>
+      <c r="AL37" s="19"/>
+      <c r="AM37" s="19"/>
+      <c r="AN37" s="19"/>
+      <c r="AO37" s="19"/>
+      <c r="AP37" s="19"/>
+      <c r="AQ37" s="19"/>
+      <c r="AR37" s="19"/>
+      <c r="AS37" s="19"/>
+      <c r="AT37" s="19"/>
+      <c r="AU37" s="19"/>
+      <c r="AV37" s="19"/>
+      <c r="AW37" s="19"/>
+      <c r="AX37" s="19"/>
+      <c r="AY37" s="19"/>
+      <c r="AZ37" s="19"/>
+      <c r="BA37" s="19"/>
+      <c r="BB37" s="19"/>
+      <c r="BC37" s="19"/>
+      <c r="BD37" s="19"/>
+      <c r="BE37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
@@ -51310,28 +51311,28 @@
       <c r="AG38" s="8"/>
       <c r="AH38" s="8"/>
       <c r="AI38" s="8"/>
-      <c r="AJ38" s="20"/>
-      <c r="AK38" s="20"/>
-      <c r="AL38" s="20"/>
-      <c r="AM38" s="20"/>
-      <c r="AN38" s="20"/>
-      <c r="AO38" s="20"/>
-      <c r="AP38" s="20"/>
-      <c r="AQ38" s="20"/>
-      <c r="AR38" s="20"/>
-      <c r="AS38" s="20"/>
-      <c r="AT38" s="20"/>
-      <c r="AU38" s="20"/>
-      <c r="AV38" s="20"/>
-      <c r="AW38" s="20"/>
-      <c r="AX38" s="20"/>
-      <c r="AY38" s="20"/>
-      <c r="AZ38" s="20"/>
-      <c r="BA38" s="20"/>
-      <c r="BB38" s="20"/>
-      <c r="BC38" s="20"/>
-      <c r="BD38" s="20"/>
-      <c r="BE38" s="20"/>
+      <c r="AJ38" s="19"/>
+      <c r="AK38" s="19"/>
+      <c r="AL38" s="19"/>
+      <c r="AM38" s="19"/>
+      <c r="AN38" s="19"/>
+      <c r="AO38" s="19"/>
+      <c r="AP38" s="19"/>
+      <c r="AQ38" s="19"/>
+      <c r="AR38" s="19"/>
+      <c r="AS38" s="19"/>
+      <c r="AT38" s="19"/>
+      <c r="AU38" s="19"/>
+      <c r="AV38" s="19"/>
+      <c r="AW38" s="19"/>
+      <c r="AX38" s="19"/>
+      <c r="AY38" s="19"/>
+      <c r="AZ38" s="19"/>
+      <c r="BA38" s="19"/>
+      <c r="BB38" s="19"/>
+      <c r="BC38" s="19"/>
+      <c r="BD38" s="19"/>
+      <c r="BE38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
@@ -51387,28 +51388,28 @@
       <c r="AG39" s="8"/>
       <c r="AH39" s="8"/>
       <c r="AI39" s="8"/>
-      <c r="AJ39" s="20"/>
-      <c r="AK39" s="20"/>
-      <c r="AL39" s="20"/>
-      <c r="AM39" s="20"/>
-      <c r="AN39" s="20"/>
-      <c r="AO39" s="20"/>
-      <c r="AP39" s="20"/>
-      <c r="AQ39" s="20"/>
-      <c r="AR39" s="20"/>
-      <c r="AS39" s="20"/>
-      <c r="AT39" s="20"/>
-      <c r="AU39" s="20"/>
-      <c r="AV39" s="20"/>
-      <c r="AW39" s="20"/>
-      <c r="AX39" s="20"/>
-      <c r="AY39" s="20"/>
-      <c r="AZ39" s="20"/>
-      <c r="BA39" s="20"/>
-      <c r="BB39" s="20"/>
-      <c r="BC39" s="20"/>
-      <c r="BD39" s="20"/>
-      <c r="BE39" s="20"/>
+      <c r="AJ39" s="19"/>
+      <c r="AK39" s="19"/>
+      <c r="AL39" s="19"/>
+      <c r="AM39" s="19"/>
+      <c r="AN39" s="19"/>
+      <c r="AO39" s="19"/>
+      <c r="AP39" s="19"/>
+      <c r="AQ39" s="19"/>
+      <c r="AR39" s="19"/>
+      <c r="AS39" s="19"/>
+      <c r="AT39" s="19"/>
+      <c r="AU39" s="19"/>
+      <c r="AV39" s="19"/>
+      <c r="AW39" s="19"/>
+      <c r="AX39" s="19"/>
+      <c r="AY39" s="19"/>
+      <c r="AZ39" s="19"/>
+      <c r="BA39" s="19"/>
+      <c r="BB39" s="19"/>
+      <c r="BC39" s="19"/>
+      <c r="BD39" s="19"/>
+      <c r="BE39" s="19"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
@@ -51461,28 +51462,28 @@
       <c r="AG40" s="8"/>
       <c r="AH40" s="8"/>
       <c r="AI40" s="8"/>
-      <c r="AJ40" s="20"/>
-      <c r="AK40" s="20"/>
-      <c r="AL40" s="20"/>
-      <c r="AM40" s="20"/>
-      <c r="AN40" s="20"/>
-      <c r="AO40" s="20"/>
-      <c r="AP40" s="20"/>
-      <c r="AQ40" s="20"/>
-      <c r="AR40" s="20"/>
-      <c r="AS40" s="20"/>
-      <c r="AT40" s="20"/>
-      <c r="AU40" s="20"/>
-      <c r="AV40" s="20"/>
-      <c r="AW40" s="20"/>
-      <c r="AX40" s="20"/>
-      <c r="AY40" s="20"/>
-      <c r="AZ40" s="20"/>
-      <c r="BA40" s="20"/>
-      <c r="BB40" s="20"/>
-      <c r="BC40" s="20"/>
-      <c r="BD40" s="20"/>
-      <c r="BE40" s="20"/>
+      <c r="AJ40" s="19"/>
+      <c r="AK40" s="19"/>
+      <c r="AL40" s="19"/>
+      <c r="AM40" s="19"/>
+      <c r="AN40" s="19"/>
+      <c r="AO40" s="19"/>
+      <c r="AP40" s="19"/>
+      <c r="AQ40" s="19"/>
+      <c r="AR40" s="19"/>
+      <c r="AS40" s="19"/>
+      <c r="AT40" s="19"/>
+      <c r="AU40" s="19"/>
+      <c r="AV40" s="19"/>
+      <c r="AW40" s="19"/>
+      <c r="AX40" s="19"/>
+      <c r="AY40" s="19"/>
+      <c r="AZ40" s="19"/>
+      <c r="BA40" s="19"/>
+      <c r="BB40" s="19"/>
+      <c r="BC40" s="19"/>
+      <c r="BD40" s="19"/>
+      <c r="BE40" s="19"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
@@ -51532,28 +51533,28 @@
       <c r="AG41" s="8"/>
       <c r="AH41" s="8"/>
       <c r="AI41" s="8"/>
-      <c r="AJ41" s="20"/>
-      <c r="AK41" s="20"/>
-      <c r="AL41" s="20"/>
-      <c r="AM41" s="20"/>
-      <c r="AN41" s="20"/>
-      <c r="AO41" s="20"/>
-      <c r="AP41" s="20"/>
-      <c r="AQ41" s="20"/>
-      <c r="AR41" s="20"/>
-      <c r="AS41" s="20"/>
-      <c r="AT41" s="20"/>
-      <c r="AU41" s="20"/>
-      <c r="AV41" s="20"/>
-      <c r="AW41" s="20"/>
-      <c r="AX41" s="20"/>
-      <c r="AY41" s="20"/>
-      <c r="AZ41" s="20"/>
-      <c r="BA41" s="20"/>
-      <c r="BB41" s="20"/>
-      <c r="BC41" s="20"/>
-      <c r="BD41" s="20"/>
-      <c r="BE41" s="20"/>
+      <c r="AJ41" s="19"/>
+      <c r="AK41" s="19"/>
+      <c r="AL41" s="19"/>
+      <c r="AM41" s="19"/>
+      <c r="AN41" s="19"/>
+      <c r="AO41" s="19"/>
+      <c r="AP41" s="19"/>
+      <c r="AQ41" s="19"/>
+      <c r="AR41" s="19"/>
+      <c r="AS41" s="19"/>
+      <c r="AT41" s="19"/>
+      <c r="AU41" s="19"/>
+      <c r="AV41" s="19"/>
+      <c r="AW41" s="19"/>
+      <c r="AX41" s="19"/>
+      <c r="AY41" s="19"/>
+      <c r="AZ41" s="19"/>
+      <c r="BA41" s="19"/>
+      <c r="BB41" s="19"/>
+      <c r="BC41" s="19"/>
+      <c r="BD41" s="19"/>
+      <c r="BE41" s="19"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
@@ -51600,28 +51601,28 @@
       <c r="AG42" s="8"/>
       <c r="AH42" s="8"/>
       <c r="AI42" s="8"/>
-      <c r="AJ42" s="20"/>
-      <c r="AK42" s="20"/>
-      <c r="AL42" s="20"/>
-      <c r="AM42" s="20"/>
-      <c r="AN42" s="20"/>
-      <c r="AO42" s="20"/>
-      <c r="AP42" s="20"/>
-      <c r="AQ42" s="20"/>
-      <c r="AR42" s="20"/>
-      <c r="AS42" s="20"/>
-      <c r="AT42" s="20"/>
-      <c r="AU42" s="20"/>
-      <c r="AV42" s="20"/>
-      <c r="AW42" s="20"/>
-      <c r="AX42" s="20"/>
-      <c r="AY42" s="20"/>
-      <c r="AZ42" s="20"/>
-      <c r="BA42" s="20"/>
-      <c r="BB42" s="20"/>
-      <c r="BC42" s="20"/>
-      <c r="BD42" s="20"/>
-      <c r="BE42" s="20"/>
+      <c r="AJ42" s="19"/>
+      <c r="AK42" s="19"/>
+      <c r="AL42" s="19"/>
+      <c r="AM42" s="19"/>
+      <c r="AN42" s="19"/>
+      <c r="AO42" s="19"/>
+      <c r="AP42" s="19"/>
+      <c r="AQ42" s="19"/>
+      <c r="AR42" s="19"/>
+      <c r="AS42" s="19"/>
+      <c r="AT42" s="19"/>
+      <c r="AU42" s="19"/>
+      <c r="AV42" s="19"/>
+      <c r="AW42" s="19"/>
+      <c r="AX42" s="19"/>
+      <c r="AY42" s="19"/>
+      <c r="AZ42" s="19"/>
+      <c r="BA42" s="19"/>
+      <c r="BB42" s="19"/>
+      <c r="BC42" s="19"/>
+      <c r="BD42" s="19"/>
+      <c r="BE42" s="19"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
@@ -51668,28 +51669,28 @@
       <c r="AG43" s="8"/>
       <c r="AH43" s="8"/>
       <c r="AI43" s="8"/>
-      <c r="AJ43" s="20"/>
-      <c r="AK43" s="20"/>
-      <c r="AL43" s="20"/>
-      <c r="AM43" s="20"/>
-      <c r="AN43" s="20"/>
-      <c r="AO43" s="20"/>
-      <c r="AP43" s="20"/>
-      <c r="AQ43" s="20"/>
-      <c r="AR43" s="20"/>
-      <c r="AS43" s="20"/>
-      <c r="AT43" s="20"/>
-      <c r="AU43" s="20"/>
-      <c r="AV43" s="20"/>
-      <c r="AW43" s="20"/>
-      <c r="AX43" s="20"/>
-      <c r="AY43" s="20"/>
-      <c r="AZ43" s="20"/>
-      <c r="BA43" s="20"/>
-      <c r="BB43" s="20"/>
-      <c r="BC43" s="20"/>
-      <c r="BD43" s="20"/>
-      <c r="BE43" s="20"/>
+      <c r="AJ43" s="19"/>
+      <c r="AK43" s="19"/>
+      <c r="AL43" s="19"/>
+      <c r="AM43" s="19"/>
+      <c r="AN43" s="19"/>
+      <c r="AO43" s="19"/>
+      <c r="AP43" s="19"/>
+      <c r="AQ43" s="19"/>
+      <c r="AR43" s="19"/>
+      <c r="AS43" s="19"/>
+      <c r="AT43" s="19"/>
+      <c r="AU43" s="19"/>
+      <c r="AV43" s="19"/>
+      <c r="AW43" s="19"/>
+      <c r="AX43" s="19"/>
+      <c r="AY43" s="19"/>
+      <c r="AZ43" s="19"/>
+      <c r="BA43" s="19"/>
+      <c r="BB43" s="19"/>
+      <c r="BC43" s="19"/>
+      <c r="BD43" s="19"/>
+      <c r="BE43" s="19"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
@@ -51736,28 +51737,28 @@
       <c r="AG44" s="8"/>
       <c r="AH44" s="8"/>
       <c r="AI44" s="8"/>
-      <c r="AJ44" s="20"/>
-      <c r="AK44" s="20"/>
-      <c r="AL44" s="20"/>
-      <c r="AM44" s="20"/>
-      <c r="AN44" s="20"/>
-      <c r="AO44" s="20"/>
-      <c r="AP44" s="20"/>
-      <c r="AQ44" s="20"/>
-      <c r="AR44" s="20"/>
-      <c r="AS44" s="20"/>
-      <c r="AT44" s="20"/>
-      <c r="AU44" s="20"/>
-      <c r="AV44" s="20"/>
-      <c r="AW44" s="20"/>
-      <c r="AX44" s="20"/>
-      <c r="AY44" s="20"/>
-      <c r="AZ44" s="20"/>
-      <c r="BA44" s="20"/>
-      <c r="BB44" s="20"/>
-      <c r="BC44" s="20"/>
-      <c r="BD44" s="20"/>
-      <c r="BE44" s="20"/>
+      <c r="AJ44" s="19"/>
+      <c r="AK44" s="19"/>
+      <c r="AL44" s="19"/>
+      <c r="AM44" s="19"/>
+      <c r="AN44" s="19"/>
+      <c r="AO44" s="19"/>
+      <c r="AP44" s="19"/>
+      <c r="AQ44" s="19"/>
+      <c r="AR44" s="19"/>
+      <c r="AS44" s="19"/>
+      <c r="AT44" s="19"/>
+      <c r="AU44" s="19"/>
+      <c r="AV44" s="19"/>
+      <c r="AW44" s="19"/>
+      <c r="AX44" s="19"/>
+      <c r="AY44" s="19"/>
+      <c r="AZ44" s="19"/>
+      <c r="BA44" s="19"/>
+      <c r="BB44" s="19"/>
+      <c r="BC44" s="19"/>
+      <c r="BD44" s="19"/>
+      <c r="BE44" s="19"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
@@ -51801,32 +51802,32 @@
       <c r="AG45" s="8"/>
       <c r="AH45" s="8"/>
       <c r="AI45" s="8"/>
-      <c r="AJ45" s="20"/>
-      <c r="AK45" s="20"/>
-      <c r="AL45" s="20"/>
-      <c r="AM45" s="20"/>
-      <c r="AN45" s="20"/>
-      <c r="AO45" s="20"/>
-      <c r="AP45" s="20"/>
-      <c r="AQ45" s="20"/>
-      <c r="AR45" s="20"/>
-      <c r="AS45" s="20"/>
-      <c r="AT45" s="20"/>
-      <c r="AU45" s="20"/>
-      <c r="AV45" s="20"/>
-      <c r="AW45" s="20"/>
-      <c r="AX45" s="20"/>
-      <c r="AY45" s="20"/>
-      <c r="AZ45" s="20"/>
-      <c r="BA45" s="20"/>
-      <c r="BB45" s="20"/>
-      <c r="BC45" s="20"/>
-      <c r="BD45" s="20"/>
-      <c r="BE45" s="20"/>
+      <c r="AJ45" s="19"/>
+      <c r="AK45" s="19"/>
+      <c r="AL45" s="19"/>
+      <c r="AM45" s="19"/>
+      <c r="AN45" s="19"/>
+      <c r="AO45" s="19"/>
+      <c r="AP45" s="19"/>
+      <c r="AQ45" s="19"/>
+      <c r="AR45" s="19"/>
+      <c r="AS45" s="19"/>
+      <c r="AT45" s="19"/>
+      <c r="AU45" s="19"/>
+      <c r="AV45" s="19"/>
+      <c r="AW45" s="19"/>
+      <c r="AX45" s="19"/>
+      <c r="AY45" s="19"/>
+      <c r="AZ45" s="19"/>
+      <c r="BA45" s="19"/>
+      <c r="BB45" s="19"/>
+      <c r="BC45" s="19"/>
+      <c r="BD45" s="19"/>
+      <c r="BE45" s="19"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>1130</v>
+        <v>1234</v>
       </c>
       <c r="B46" s="15" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -51866,28 +51867,28 @@
       <c r="AG46" s="8"/>
       <c r="AH46" s="8"/>
       <c r="AI46" s="8"/>
-      <c r="AJ46" s="20"/>
-      <c r="AK46" s="20"/>
-      <c r="AL46" s="20"/>
-      <c r="AM46" s="20"/>
-      <c r="AN46" s="20"/>
-      <c r="AO46" s="20"/>
-      <c r="AP46" s="20"/>
-      <c r="AQ46" s="20"/>
-      <c r="AR46" s="20"/>
-      <c r="AS46" s="20"/>
-      <c r="AT46" s="20"/>
-      <c r="AU46" s="20"/>
-      <c r="AV46" s="20"/>
-      <c r="AW46" s="20"/>
-      <c r="AX46" s="20"/>
-      <c r="AY46" s="20"/>
-      <c r="AZ46" s="20"/>
-      <c r="BA46" s="20"/>
-      <c r="BB46" s="20"/>
-      <c r="BC46" s="20"/>
-      <c r="BD46" s="20"/>
-      <c r="BE46" s="20"/>
+      <c r="AJ46" s="19"/>
+      <c r="AK46" s="19"/>
+      <c r="AL46" s="19"/>
+      <c r="AM46" s="19"/>
+      <c r="AN46" s="19"/>
+      <c r="AO46" s="19"/>
+      <c r="AP46" s="19"/>
+      <c r="AQ46" s="19"/>
+      <c r="AR46" s="19"/>
+      <c r="AS46" s="19"/>
+      <c r="AT46" s="19"/>
+      <c r="AU46" s="19"/>
+      <c r="AV46" s="19"/>
+      <c r="AW46" s="19"/>
+      <c r="AX46" s="19"/>
+      <c r="AY46" s="19"/>
+      <c r="AZ46" s="19"/>
+      <c r="BA46" s="19"/>
+      <c r="BB46" s="19"/>
+      <c r="BC46" s="19"/>
+      <c r="BD46" s="19"/>
+      <c r="BE46" s="19"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
@@ -51931,28 +51932,28 @@
       <c r="AG47" s="9"/>
       <c r="AH47" s="9"/>
       <c r="AI47" s="9"/>
-      <c r="AJ47" s="20"/>
-      <c r="AK47" s="20"/>
-      <c r="AL47" s="20"/>
-      <c r="AM47" s="20"/>
-      <c r="AN47" s="20"/>
-      <c r="AO47" s="20"/>
-      <c r="AP47" s="20"/>
-      <c r="AQ47" s="20"/>
-      <c r="AR47" s="20"/>
-      <c r="AS47" s="20"/>
-      <c r="AT47" s="20"/>
-      <c r="AU47" s="20"/>
-      <c r="AV47" s="20"/>
-      <c r="AW47" s="20"/>
-      <c r="AX47" s="20"/>
-      <c r="AY47" s="20"/>
-      <c r="AZ47" s="20"/>
-      <c r="BA47" s="20"/>
-      <c r="BB47" s="20"/>
-      <c r="BC47" s="20"/>
-      <c r="BD47" s="20"/>
-      <c r="BE47" s="20"/>
+      <c r="AJ47" s="19"/>
+      <c r="AK47" s="19"/>
+      <c r="AL47" s="19"/>
+      <c r="AM47" s="19"/>
+      <c r="AN47" s="19"/>
+      <c r="AO47" s="19"/>
+      <c r="AP47" s="19"/>
+      <c r="AQ47" s="19"/>
+      <c r="AR47" s="19"/>
+      <c r="AS47" s="19"/>
+      <c r="AT47" s="19"/>
+      <c r="AU47" s="19"/>
+      <c r="AV47" s="19"/>
+      <c r="AW47" s="19"/>
+      <c r="AX47" s="19"/>
+      <c r="AY47" s="19"/>
+      <c r="AZ47" s="19"/>
+      <c r="BA47" s="19"/>
+      <c r="BB47" s="19"/>
+      <c r="BC47" s="19"/>
+      <c r="BD47" s="19"/>
+      <c r="BE47" s="19"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
@@ -57489,7 +57490,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="8" t="s">
-        <v>1161</v>
+        <v>1235</v>
       </c>
       <c r="B146" s="15" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -63398,8 +63399,8 @@
   </sheetPr>
   <dimension ref="A1:O164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L50" activeCellId="0" sqref="L50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -63451,7 +63452,7 @@
         <v>1015</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>1233</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64097,7 +64098,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>1017</v>
+        <v>1233</v>
       </c>
       <c r="B15" s="8" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -67670,7 +67671,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="8" t="s">
-        <v>1130</v>
+        <v>1234</v>
       </c>
       <c r="B138" s="8" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>
@@ -67845,7 +67846,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="8" t="s">
-        <v>1161</v>
+        <v>1235</v>
       </c>
       <c r="B145" s="8" t="e">
         <f aca="false">VLOOKUP(A:A,Database!B:C,2,0)</f>

</xml_diff>